<commit_message>
Valores corretos na planilha de cs
</commit_message>
<xml_diff>
--- a/Data base definitivo.xlsx
+++ b/Data base definitivo.xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\Programação\Trabalho\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685C1115-682A-4195-A146-9BDD413EE88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7815"/>
+    <workbookView xWindow="-6750" yWindow="435" windowWidth="14670" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
   <si>
     <t>data</t>
   </si>
@@ -523,39 +539,6 @@
     <t>ganhos_cs</t>
   </si>
   <si>
-    <t>222538.77</t>
-  </si>
-  <si>
-    <t>1461869.54</t>
-  </si>
-  <si>
-    <t>2712515.01</t>
-  </si>
-  <si>
-    <t>7034970.14</t>
-  </si>
-  <si>
-    <t>19828410.90</t>
-  </si>
-  <si>
-    <t>21706143.07</t>
-  </si>
-  <si>
-    <t>25578825.95</t>
-  </si>
-  <si>
-    <t>24641880.12</t>
-  </si>
-  <si>
-    <t>16625485.72</t>
-  </si>
-  <si>
-    <t>21319818.54</t>
-  </si>
-  <si>
-    <t>3855347.08</t>
-  </si>
-  <si>
     <t>variação</t>
   </si>
   <si>
@@ -569,13 +552,16 @@
   </si>
   <si>
     <t>mdaplayer</t>
+  </si>
+  <si>
+    <t>6340704.98</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,7 +573,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -620,6 +606,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -641,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,6 +651,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,7 +717,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -771,7 +769,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -965,26 +963,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE116" sqref="AE116"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="U145" sqref="U145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" style="16" customWidth="1"/>
+    <col min="22" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1048,23 +1049,23 @@
       <c r="T1" t="s">
         <v>167</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="16" t="s">
         <v>168</v>
       </c>
       <c r="V1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="W1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="X1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="Y1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="Z1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -1128,7 +1129,7 @@
       <c r="T2">
         <v>0</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="14">
         <v>0</v>
       </c>
       <c r="V2">
@@ -1208,7 +1209,7 @@
       <c r="T3">
         <v>0</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="15">
         <v>0</v>
       </c>
       <c r="V3">
@@ -1288,7 +1289,7 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="15">
         <v>0</v>
       </c>
       <c r="V4">
@@ -1368,7 +1369,7 @@
       <c r="T5">
         <v>0</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="15">
         <v>0</v>
       </c>
       <c r="V5">
@@ -1448,7 +1449,7 @@
       <c r="T6">
         <v>0</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="15">
         <v>0</v>
       </c>
       <c r="V6">
@@ -1528,7 +1529,7 @@
       <c r="T7">
         <v>0</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="15">
         <v>0</v>
       </c>
       <c r="V7">
@@ -1608,7 +1609,7 @@
       <c r="T8">
         <v>0</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="15">
         <v>0</v>
       </c>
       <c r="V8">
@@ -1688,7 +1689,7 @@
       <c r="T9">
         <v>0</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="15">
         <v>0</v>
       </c>
       <c r="V9">
@@ -1768,7 +1769,7 @@
       <c r="T10">
         <v>0</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="15">
         <v>0</v>
       </c>
       <c r="V10">
@@ -1848,7 +1849,7 @@
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="15">
         <v>0</v>
       </c>
       <c r="V11">
@@ -1928,7 +1929,7 @@
       <c r="T12">
         <v>0</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="15">
         <v>0</v>
       </c>
       <c r="V12">
@@ -2008,7 +2009,7 @@
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="15">
         <v>0</v>
       </c>
       <c r="V13">
@@ -2088,7 +2089,7 @@
       <c r="T14">
         <v>0</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="15">
         <v>0</v>
       </c>
       <c r="V14">
@@ -2168,7 +2169,7 @@
       <c r="T15">
         <v>0</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="15">
         <v>0</v>
       </c>
       <c r="V15">
@@ -2248,7 +2249,7 @@
       <c r="T16">
         <v>0</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="15">
         <v>0</v>
       </c>
       <c r="V16">
@@ -2328,7 +2329,7 @@
       <c r="T17">
         <v>0</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="15">
         <v>0</v>
       </c>
       <c r="V17">
@@ -2408,7 +2409,7 @@
       <c r="T18">
         <v>0</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="15">
         <v>0</v>
       </c>
       <c r="V18">
@@ -2488,7 +2489,7 @@
       <c r="T19">
         <v>0</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="15">
         <v>0</v>
       </c>
       <c r="V19">
@@ -2568,7 +2569,7 @@
       <c r="T20">
         <v>0</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="15">
         <v>0</v>
       </c>
       <c r="V20">
@@ -2648,7 +2649,7 @@
       <c r="T21">
         <v>0</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="15">
         <v>0</v>
       </c>
       <c r="V21">
@@ -2728,7 +2729,7 @@
       <c r="T22">
         <v>0</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="15">
         <v>0</v>
       </c>
       <c r="V22">
@@ -2808,7 +2809,7 @@
       <c r="T23">
         <v>0</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="15">
         <v>0</v>
       </c>
       <c r="V23">
@@ -2888,7 +2889,7 @@
       <c r="T24">
         <v>0</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="15">
         <v>0</v>
       </c>
       <c r="V24">
@@ -2968,7 +2969,7 @@
       <c r="T25">
         <v>0</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="15">
         <v>0</v>
       </c>
       <c r="V25">
@@ -3048,8 +3049,8 @@
       <c r="T26">
         <v>0</v>
       </c>
-      <c r="U26" t="s">
-        <v>169</v>
+      <c r="U26" s="15">
+        <v>0</v>
       </c>
       <c r="V26">
         <v>0</v>
@@ -3128,8 +3129,8 @@
       <c r="T27">
         <v>0</v>
       </c>
-      <c r="U27" t="s">
-        <v>169</v>
+      <c r="U27" s="15">
+        <v>0</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -3208,8 +3209,8 @@
       <c r="T28">
         <v>0</v>
       </c>
-      <c r="U28" t="s">
-        <v>169</v>
+      <c r="U28" s="15">
+        <v>0</v>
       </c>
       <c r="V28">
         <v>0</v>
@@ -3288,8 +3289,8 @@
       <c r="T29">
         <v>0</v>
       </c>
-      <c r="U29" t="s">
-        <v>169</v>
+      <c r="U29" s="14">
+        <v>1309.33</v>
       </c>
       <c r="V29">
         <v>0</v>
@@ -3368,8 +3369,8 @@
       <c r="T30">
         <v>0</v>
       </c>
-      <c r="U30" t="s">
-        <v>169</v>
+      <c r="U30" s="14">
+        <v>0</v>
       </c>
       <c r="V30">
         <v>0</v>
@@ -3448,8 +3449,8 @@
       <c r="T31">
         <v>0</v>
       </c>
-      <c r="U31" t="s">
-        <v>169</v>
+      <c r="U31" s="14">
+        <v>0</v>
       </c>
       <c r="V31">
         <v>0</v>
@@ -3528,8 +3529,8 @@
       <c r="T32">
         <v>0</v>
       </c>
-      <c r="U32" t="s">
-        <v>169</v>
+      <c r="U32" s="14">
+        <v>0</v>
       </c>
       <c r="V32">
         <v>0</v>
@@ -3608,8 +3609,8 @@
       <c r="T33">
         <v>0</v>
       </c>
-      <c r="U33" t="s">
-        <v>169</v>
+      <c r="U33" s="15">
+        <v>6772.76</v>
       </c>
       <c r="V33">
         <v>0</v>
@@ -3688,8 +3689,8 @@
       <c r="T34">
         <v>0</v>
       </c>
-      <c r="U34" t="s">
-        <v>169</v>
+      <c r="U34" s="15">
+        <v>13260.77</v>
       </c>
       <c r="V34">
         <v>0</v>
@@ -3768,8 +3769,8 @@
       <c r="T35">
         <v>0</v>
       </c>
-      <c r="U35" t="s">
-        <v>169</v>
+      <c r="U35" s="15">
+        <v>23973.98</v>
       </c>
       <c r="V35">
         <v>0</v>
@@ -3848,8 +3849,8 @@
       <c r="T36">
         <v>0</v>
       </c>
-      <c r="U36" t="s">
-        <v>169</v>
+      <c r="U36" s="15">
+        <v>122425.32</v>
       </c>
       <c r="V36">
         <v>0</v>
@@ -3928,8 +3929,8 @@
       <c r="T37">
         <v>0</v>
       </c>
-      <c r="U37" t="s">
-        <v>169</v>
+      <c r="U37" s="15">
+        <v>222538.77</v>
       </c>
       <c r="V37">
         <v>0</v>
@@ -4008,8 +4009,8 @@
       <c r="T38">
         <v>0</v>
       </c>
-      <c r="U38" t="s">
-        <v>170</v>
+      <c r="U38" s="15">
+        <v>21889.65</v>
       </c>
       <c r="V38">
         <v>0</v>
@@ -4088,8 +4089,8 @@
       <c r="T39">
         <v>0</v>
       </c>
-      <c r="U39" t="s">
-        <v>170</v>
+      <c r="U39" s="15">
+        <v>71698.91</v>
       </c>
       <c r="V39">
         <v>0</v>
@@ -4168,8 +4169,8 @@
       <c r="T40">
         <v>0</v>
       </c>
-      <c r="U40" t="s">
-        <v>170</v>
+      <c r="U40" s="15">
+        <v>164820.20000000001</v>
       </c>
       <c r="V40">
         <v>0</v>
@@ -4248,8 +4249,8 @@
       <c r="T41">
         <v>0</v>
       </c>
-      <c r="U41" t="s">
-        <v>170</v>
+      <c r="U41" s="15">
+        <v>297748.49</v>
       </c>
       <c r="V41">
         <v>0</v>
@@ -4328,8 +4329,8 @@
       <c r="T42">
         <v>0</v>
       </c>
-      <c r="U42" t="s">
-        <v>170</v>
+      <c r="U42" s="15">
+        <v>332547.96000000002</v>
       </c>
       <c r="V42">
         <v>0</v>
@@ -4408,8 +4409,8 @@
       <c r="T43">
         <v>0</v>
       </c>
-      <c r="U43" t="s">
-        <v>170</v>
+      <c r="U43" s="15">
+        <v>482987.23</v>
       </c>
       <c r="V43">
         <v>0</v>
@@ -4488,8 +4489,8 @@
       <c r="T44">
         <v>0</v>
       </c>
-      <c r="U44" t="s">
-        <v>170</v>
+      <c r="U44" s="15">
+        <v>520402.96</v>
       </c>
       <c r="V44">
         <v>0</v>
@@ -4568,8 +4569,8 @@
       <c r="T45">
         <v>0</v>
       </c>
-      <c r="U45" t="s">
-        <v>170</v>
+      <c r="U45" s="15">
+        <v>591825.81999999995</v>
       </c>
       <c r="V45">
         <v>0</v>
@@ -4648,8 +4649,8 @@
       <c r="T46">
         <v>0</v>
       </c>
-      <c r="U46" t="s">
-        <v>170</v>
+      <c r="U46" s="15">
+        <v>648901.71</v>
       </c>
       <c r="V46">
         <v>0</v>
@@ -4728,8 +4729,8 @@
       <c r="T47">
         <v>0</v>
       </c>
-      <c r="U47" t="s">
-        <v>170</v>
+      <c r="U47" s="15">
+        <v>731668.88</v>
       </c>
       <c r="V47">
         <v>0</v>
@@ -4808,8 +4809,8 @@
       <c r="T48">
         <v>0</v>
       </c>
-      <c r="U48" t="s">
-        <v>170</v>
+      <c r="U48" s="15">
+        <v>1331452.76</v>
       </c>
       <c r="V48">
         <v>0</v>
@@ -4888,8 +4889,8 @@
       <c r="T49">
         <v>0</v>
       </c>
-      <c r="U49" t="s">
-        <v>170</v>
+      <c r="U49" s="15">
+        <v>1461869.54</v>
       </c>
       <c r="V49">
         <v>0</v>
@@ -4968,8 +4969,8 @@
       <c r="T50">
         <v>0</v>
       </c>
-      <c r="U50" t="s">
-        <v>171</v>
+      <c r="U50" s="15">
+        <v>81389.25</v>
       </c>
       <c r="V50">
         <v>0</v>
@@ -5048,8 +5049,8 @@
       <c r="T51">
         <v>0</v>
       </c>
-      <c r="U51" t="s">
-        <v>171</v>
+      <c r="U51" s="15">
+        <v>122770.38</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -5128,8 +5129,8 @@
       <c r="T52">
         <v>0</v>
       </c>
-      <c r="U52" t="s">
-        <v>171</v>
+      <c r="U52" s="15">
+        <v>669657.65</v>
       </c>
       <c r="V52">
         <v>0</v>
@@ -5208,8 +5209,8 @@
       <c r="T53">
         <v>0</v>
       </c>
-      <c r="U53" t="s">
-        <v>171</v>
+      <c r="U53" s="15">
+        <v>754716.57</v>
       </c>
       <c r="V53">
         <v>0</v>
@@ -5288,8 +5289,8 @@
       <c r="T54">
         <v>0</v>
       </c>
-      <c r="U54" t="s">
-        <v>171</v>
+      <c r="U54" s="15">
+        <v>816811.22</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -5368,8 +5369,8 @@
       <c r="T55">
         <v>0</v>
       </c>
-      <c r="U55" t="s">
-        <v>171</v>
+      <c r="U55" s="15">
+        <v>971753.74</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -5448,8 +5449,8 @@
       <c r="T56">
         <v>0</v>
       </c>
-      <c r="U56" t="s">
-        <v>171</v>
+      <c r="U56" s="15">
+        <v>1038665.2</v>
       </c>
       <c r="V56">
         <v>0</v>
@@ -5528,8 +5529,8 @@
       <c r="T57">
         <v>0</v>
       </c>
-      <c r="U57" t="s">
-        <v>171</v>
+      <c r="U57" s="15">
+        <v>1645629.14</v>
       </c>
       <c r="V57">
         <v>0</v>
@@ -5608,8 +5609,8 @@
       <c r="T58">
         <v>0</v>
       </c>
-      <c r="U58" t="s">
-        <v>171</v>
+      <c r="U58" s="15">
+        <v>1707689.43</v>
       </c>
       <c r="V58">
         <v>0</v>
@@ -5688,8 +5689,8 @@
       <c r="T59">
         <v>0</v>
       </c>
-      <c r="U59" t="s">
-        <v>171</v>
+      <c r="U59" s="15">
+        <v>1923818.96</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -5768,8 +5769,8 @@
       <c r="T60">
         <v>0</v>
       </c>
-      <c r="U60" t="s">
-        <v>171</v>
+      <c r="U60" s="15">
+        <v>2571492.64</v>
       </c>
       <c r="V60">
         <v>0</v>
@@ -5848,8 +5849,8 @@
       <c r="T61">
         <v>0</v>
       </c>
-      <c r="U61" t="s">
-        <v>171</v>
+      <c r="U61" s="15">
+        <v>2712515.01</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -5928,8 +5929,8 @@
       <c r="T62">
         <v>0</v>
       </c>
-      <c r="U62" t="s">
-        <v>172</v>
+      <c r="U62" s="15">
+        <v>109366.62</v>
       </c>
       <c r="V62">
         <v>0</v>
@@ -6008,8 +6009,8 @@
       <c r="T63">
         <v>0</v>
       </c>
-      <c r="U63" t="s">
-        <v>172</v>
+      <c r="U63" s="15">
+        <v>219315.47</v>
       </c>
       <c r="V63">
         <v>0</v>
@@ -6088,8 +6089,8 @@
       <c r="T64">
         <v>0</v>
       </c>
-      <c r="U64" t="s">
-        <v>172</v>
+      <c r="U64" s="15">
+        <v>882518.74</v>
       </c>
       <c r="V64">
         <v>0</v>
@@ -6168,8 +6169,8 @@
       <c r="T65">
         <v>0</v>
       </c>
-      <c r="U65" t="s">
-        <v>172</v>
+      <c r="U65" s="15">
+        <v>1355408.95</v>
       </c>
       <c r="V65">
         <v>0</v>
@@ -6248,8 +6249,8 @@
       <c r="T66">
         <v>0</v>
       </c>
-      <c r="U66" t="s">
-        <v>172</v>
+      <c r="U66" s="15">
+        <v>1609173.1</v>
       </c>
       <c r="V66">
         <v>0</v>
@@ -6328,8 +6329,8 @@
       <c r="T67">
         <v>0</v>
       </c>
-      <c r="U67" t="s">
-        <v>172</v>
+      <c r="U67" s="15">
+        <v>2226852.1800000002</v>
       </c>
       <c r="V67">
         <v>0</v>
@@ -6408,8 +6409,8 @@
       <c r="T68">
         <v>0</v>
       </c>
-      <c r="U68" t="s">
-        <v>172</v>
+      <c r="U68" s="15">
+        <v>3107961.9</v>
       </c>
       <c r="V68">
         <v>0</v>
@@ -6488,8 +6489,8 @@
       <c r="T69">
         <v>0</v>
       </c>
-      <c r="U69" t="s">
-        <v>172</v>
+      <c r="U69" s="15">
+        <v>3855994.04</v>
       </c>
       <c r="V69">
         <v>0</v>
@@ -6568,8 +6569,8 @@
       <c r="T70">
         <v>0</v>
       </c>
-      <c r="U70" t="s">
-        <v>172</v>
+      <c r="U70" s="15">
+        <v>4431774.63</v>
       </c>
       <c r="V70">
         <v>0</v>
@@ -6648,8 +6649,8 @@
       <c r="T71">
         <v>0</v>
       </c>
-      <c r="U71" t="s">
-        <v>172</v>
+      <c r="U71" s="15">
+        <v>4846558.66</v>
       </c>
       <c r="V71">
         <v>0</v>
@@ -6728,8 +6729,8 @@
       <c r="T72">
         <v>0</v>
       </c>
-      <c r="U72" t="s">
-        <v>172</v>
+      <c r="U72" s="15">
+        <v>6040571.0499999998</v>
       </c>
       <c r="V72">
         <v>0</v>
@@ -6808,8 +6809,8 @@
       <c r="T73">
         <v>0</v>
       </c>
-      <c r="U73" t="s">
-        <v>172</v>
+      <c r="U73" s="15">
+        <v>7343809.6799999997</v>
       </c>
       <c r="V73">
         <v>0</v>
@@ -6888,8 +6889,8 @@
       <c r="T74">
         <v>0</v>
       </c>
-      <c r="U74" t="s">
-        <v>173</v>
+      <c r="U74" s="15">
+        <v>703550.83</v>
       </c>
       <c r="V74">
         <v>0</v>
@@ -6968,8 +6969,8 @@
       <c r="T75">
         <v>0</v>
       </c>
-      <c r="U75" t="s">
-        <v>173</v>
+      <c r="U75" s="15">
+        <v>1312413.95</v>
       </c>
       <c r="V75">
         <v>0</v>
@@ -7048,8 +7049,8 @@
       <c r="T76">
         <v>0</v>
       </c>
-      <c r="U76" t="s">
-        <v>173</v>
+      <c r="U76" s="15">
+        <v>1789987.13</v>
       </c>
       <c r="V76">
         <v>0</v>
@@ -7128,8 +7129,8 @@
       <c r="T77">
         <v>0</v>
       </c>
-      <c r="U77" t="s">
-        <v>173</v>
+      <c r="U77" s="15">
+        <v>4378457.7699999996</v>
       </c>
       <c r="V77">
         <v>0</v>
@@ -7208,8 +7209,8 @@
       <c r="T78">
         <v>0</v>
       </c>
-      <c r="U78" t="s">
-        <v>173</v>
+      <c r="U78" s="15">
+        <v>5960841.9400000004</v>
       </c>
       <c r="V78">
         <v>0</v>
@@ -7288,8 +7289,8 @@
       <c r="T79">
         <v>0</v>
       </c>
-      <c r="U79" t="s">
-        <v>173</v>
+      <c r="U79" s="15">
+        <v>7203783.9299999997</v>
       </c>
       <c r="V79">
         <v>0</v>
@@ -7368,8 +7369,8 @@
       <c r="T80">
         <v>0</v>
       </c>
-      <c r="U80" t="s">
-        <v>173</v>
+      <c r="U80" s="15">
+        <v>11128892.18</v>
       </c>
       <c r="V80">
         <v>0</v>
@@ -7448,8 +7449,8 @@
       <c r="T81">
         <v>0</v>
       </c>
-      <c r="U81" t="s">
-        <v>173</v>
+      <c r="U81" s="15">
+        <v>11572328.16</v>
       </c>
       <c r="V81">
         <v>0</v>
@@ -7528,8 +7529,8 @@
       <c r="T82">
         <v>0</v>
       </c>
-      <c r="U82" t="s">
-        <v>173</v>
+      <c r="U82" s="15">
+        <v>12551395.25</v>
       </c>
       <c r="V82">
         <v>0</v>
@@ -7608,8 +7609,8 @@
       <c r="T83">
         <v>0</v>
       </c>
-      <c r="U83" t="s">
-        <v>173</v>
+      <c r="U83" s="15">
+        <v>14874091.83</v>
       </c>
       <c r="V83">
         <v>0</v>
@@ -7688,8 +7689,8 @@
       <c r="T84">
         <v>0</v>
       </c>
-      <c r="U84" t="s">
-        <v>173</v>
+      <c r="U84" s="15">
+        <v>16594388.42</v>
       </c>
       <c r="V84">
         <v>0</v>
@@ -7768,8 +7769,8 @@
       <c r="T85">
         <v>22.3</v>
       </c>
-      <c r="U85" t="s">
-        <v>173</v>
+      <c r="U85" s="15">
+        <v>19828410.899999999</v>
       </c>
       <c r="V85">
         <v>0</v>
@@ -7848,8 +7849,8 @@
       <c r="T86">
         <v>0.2</v>
       </c>
-      <c r="U86" t="s">
-        <v>174</v>
+      <c r="U86" s="15">
+        <v>3674065.16</v>
       </c>
       <c r="V86">
         <v>0</v>
@@ -7928,8 +7929,8 @@
       <c r="T87">
         <v>-8.6</v>
       </c>
-      <c r="U87" t="s">
-        <v>174</v>
+      <c r="U87" s="15">
+        <v>4222397.51</v>
       </c>
       <c r="V87">
         <v>0</v>
@@ -8008,8 +8009,8 @@
       <c r="T88">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="U88" t="s">
-        <v>174</v>
+      <c r="U88" s="15">
+        <v>4653798.38</v>
       </c>
       <c r="V88">
         <v>0</v>
@@ -8088,8 +8089,8 @@
       <c r="T89">
         <v>5</v>
       </c>
-      <c r="U89" t="s">
-        <v>174</v>
+      <c r="U89" s="15">
+        <v>5431545.3600000003</v>
       </c>
       <c r="V89">
         <v>0</v>
@@ -8168,8 +8169,8 @@
       <c r="T90">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="U90" t="s">
-        <v>174</v>
+      <c r="U90" s="15">
+        <v>6255335.6500000004</v>
       </c>
       <c r="V90">
         <v>0</v>
@@ -8248,8 +8249,8 @@
       <c r="T91">
         <v>0</v>
       </c>
-      <c r="U91" t="s">
-        <v>174</v>
+      <c r="U91" s="15">
+        <v>9066567.9100000001</v>
       </c>
       <c r="V91">
         <v>0</v>
@@ -8328,8 +8329,8 @@
       <c r="T92">
         <v>-15.1</v>
       </c>
-      <c r="U92" t="s">
-        <v>174</v>
+      <c r="U92" s="15">
+        <v>11881322.24</v>
       </c>
       <c r="V92">
         <v>0</v>
@@ -8408,8 +8409,8 @@
       <c r="T93">
         <v>3.5</v>
       </c>
-      <c r="U93" t="s">
-        <v>174</v>
+      <c r="U93" s="15">
+        <v>12177797.380000001</v>
       </c>
       <c r="V93">
         <v>0</v>
@@ -8488,8 +8489,8 @@
       <c r="T94">
         <v>27.2</v>
       </c>
-      <c r="U94" t="s">
-        <v>174</v>
+      <c r="U94" s="15">
+        <v>13517829.67</v>
       </c>
       <c r="V94">
         <v>0</v>
@@ -8568,8 +8569,8 @@
       <c r="T95">
         <v>-12.4</v>
       </c>
-      <c r="U95" t="s">
-        <v>174</v>
+      <c r="U95" s="15">
+        <v>15955291.33</v>
       </c>
       <c r="V95">
         <v>0</v>
@@ -8648,8 +8649,8 @@
       <c r="T96">
         <v>-16</v>
       </c>
-      <c r="U96" t="s">
-        <v>174</v>
+      <c r="U96" s="15">
+        <v>17789627.760000002</v>
       </c>
       <c r="V96">
         <v>0</v>
@@ -8728,8 +8729,8 @@
       <c r="T97">
         <v>28</v>
       </c>
-      <c r="U97" t="s">
-        <v>174</v>
+      <c r="U97" s="15">
+        <v>21706143.07</v>
       </c>
       <c r="V97">
         <v>0</v>
@@ -8808,8 +8809,8 @@
       <c r="T98">
         <v>-9</v>
       </c>
-      <c r="U98" t="s">
-        <v>175</v>
+      <c r="U98" s="15">
+        <v>2269332.4</v>
       </c>
       <c r="V98">
         <v>0</v>
@@ -8888,8 +8889,8 @@
       <c r="T99">
         <v>9.6999999999999993</v>
       </c>
-      <c r="U99" t="s">
-        <v>175</v>
+      <c r="U99" s="15">
+        <v>3051946.94</v>
       </c>
       <c r="V99">
         <v>0</v>
@@ -8968,8 +8969,8 @@
       <c r="T100">
         <v>-16.5</v>
       </c>
-      <c r="U100" t="s">
-        <v>175</v>
+      <c r="U100" s="15">
+        <v>6343374.9900000002</v>
       </c>
       <c r="V100">
         <v>0</v>
@@ -9048,8 +9049,8 @@
       <c r="T101">
         <v>10.6</v>
       </c>
-      <c r="U101" t="s">
-        <v>175</v>
+      <c r="U101" s="15">
+        <v>7175581.3899999997</v>
       </c>
       <c r="V101">
         <v>0</v>
@@ -9128,8 +9129,8 @@
       <c r="T102">
         <v>-11.7</v>
       </c>
-      <c r="U102" t="s">
-        <v>175</v>
+      <c r="U102" s="15">
+        <v>9033439.8599999994</v>
       </c>
       <c r="V102">
         <v>0</v>
@@ -9208,8 +9209,8 @@
       <c r="T103">
         <v>3.5</v>
       </c>
-      <c r="U103" t="s">
-        <v>175</v>
+      <c r="U103" s="15">
+        <v>11085702.880000001</v>
       </c>
       <c r="V103">
         <v>0</v>
@@ -9288,8 +9289,8 @@
       <c r="T104">
         <v>8.4</v>
       </c>
-      <c r="U104" t="s">
-        <v>175</v>
+      <c r="U104" s="15">
+        <v>13103512.65</v>
       </c>
       <c r="V104">
         <v>0</v>
@@ -9368,8 +9369,8 @@
       <c r="T105">
         <v>-5.8</v>
       </c>
-      <c r="U105" t="s">
-        <v>175</v>
+      <c r="U105" s="15">
+        <v>14056493.49</v>
       </c>
       <c r="V105">
         <v>0</v>
@@ -9448,8 +9449,8 @@
       <c r="T106">
         <v>42.4</v>
       </c>
-      <c r="U106" t="s">
-        <v>175</v>
+      <c r="U106" s="15">
+        <v>17472086.800000001</v>
       </c>
       <c r="V106">
         <v>0</v>
@@ -9528,8 +9529,8 @@
       <c r="T107">
         <v>-22.4</v>
       </c>
-      <c r="U107" t="s">
-        <v>175</v>
+      <c r="U107" s="15">
+        <v>18934213.420000002</v>
       </c>
       <c r="V107">
         <v>0</v>
@@ -9608,8 +9609,8 @@
       <c r="T108">
         <v>-14.7</v>
       </c>
-      <c r="U108" t="s">
-        <v>175</v>
+      <c r="U108" s="15">
+        <v>20983098.93</v>
       </c>
       <c r="V108">
         <v>0</v>
@@ -9688,8 +9689,8 @@
       <c r="T109">
         <v>37.5</v>
       </c>
-      <c r="U109" t="s">
-        <v>175</v>
+      <c r="U109" s="15">
+        <v>25578825.949999999</v>
       </c>
       <c r="V109">
         <v>0</v>
@@ -9768,8 +9769,8 @@
       <c r="T110">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="U110" t="s">
-        <v>176</v>
+      <c r="U110" s="15">
+        <v>853086.74</v>
       </c>
       <c r="V110">
         <v>0</v>
@@ -9848,8 +9849,8 @@
       <c r="T111">
         <v>14.1</v>
       </c>
-      <c r="U111" t="s">
-        <v>176</v>
+      <c r="U111" s="15">
+        <v>1085693.5</v>
       </c>
       <c r="V111">
         <v>0</v>
@@ -9928,8 +9929,8 @@
       <c r="T112">
         <v>-14.7</v>
       </c>
-      <c r="U112" t="s">
-        <v>176</v>
+      <c r="U112" s="15">
+        <v>4484567.3499999996</v>
       </c>
       <c r="V112">
         <v>0</v>
@@ -10008,8 +10009,8 @@
       <c r="T113">
         <v>11.2</v>
       </c>
-      <c r="U113" t="s">
-        <v>176</v>
+      <c r="U113" s="15">
+        <v>6143408.9000000004</v>
       </c>
       <c r="V113">
         <v>0</v>
@@ -10088,8 +10089,8 @@
       <c r="T114">
         <v>-13.3</v>
       </c>
-      <c r="U114" t="s">
-        <v>176</v>
+      <c r="U114" s="15">
+        <v>7108982.2599999998</v>
       </c>
       <c r="V114">
         <v>0</v>
@@ -10168,8 +10169,8 @@
       <c r="T115">
         <v>-23.5</v>
       </c>
-      <c r="U115" t="s">
-        <v>176</v>
+      <c r="U115" s="15">
+        <v>9665600.8200000003</v>
       </c>
       <c r="V115">
         <v>0</v>
@@ -10248,8 +10249,8 @@
       <c r="T116">
         <v>26.2</v>
       </c>
-      <c r="U116" t="s">
-        <v>176</v>
+      <c r="U116" s="15">
+        <v>12538772.5</v>
       </c>
       <c r="V116">
         <v>0</v>
@@ -10328,8 +10329,8 @@
       <c r="T117">
         <v>-9.9</v>
       </c>
-      <c r="U117" t="s">
-        <v>176</v>
+      <c r="U117" s="15">
+        <v>12769762.66</v>
       </c>
       <c r="V117">
         <v>0</v>
@@ -10408,8 +10409,8 @@
       <c r="T118">
         <v>56.2</v>
       </c>
-      <c r="U118" t="s">
-        <v>176</v>
+      <c r="U118" s="15">
+        <v>15917600.130000001</v>
       </c>
       <c r="V118">
         <v>0</v>
@@ -10488,8 +10489,8 @@
       <c r="T119">
         <v>-24.2</v>
       </c>
-      <c r="U119" t="s">
-        <v>176</v>
+      <c r="U119" s="15">
+        <v>17238507.620000001</v>
       </c>
       <c r="V119">
         <v>0</v>
@@ -10568,8 +10569,8 @@
       <c r="T120">
         <v>-14.4</v>
       </c>
-      <c r="U120" t="s">
-        <v>176</v>
+      <c r="U120" s="15">
+        <v>18919910.899999999</v>
       </c>
       <c r="V120">
         <v>0</v>
@@ -10648,8 +10649,8 @@
       <c r="T121">
         <v>27</v>
       </c>
-      <c r="U121" t="s">
-        <v>176</v>
+      <c r="U121" s="15">
+        <v>24410889.960000001</v>
       </c>
       <c r="V121">
         <v>0</v>
@@ -10728,8 +10729,8 @@
       <c r="T122">
         <v>21.7</v>
       </c>
-      <c r="U122" t="s">
-        <v>177</v>
+      <c r="U122" s="15">
+        <v>351510.31</v>
       </c>
       <c r="V122">
         <v>12900</v>
@@ -10808,8 +10809,8 @@
       <c r="T123">
         <v>1.7</v>
       </c>
-      <c r="U123" t="s">
-        <v>177</v>
+      <c r="U123" s="15">
+        <v>856920.23</v>
       </c>
       <c r="V123">
         <v>130000</v>
@@ -10888,8 +10889,8 @@
       <c r="T124">
         <v>9.6</v>
       </c>
-      <c r="U124" t="s">
-        <v>177</v>
+      <c r="U124" s="15">
+        <v>1418856.88</v>
       </c>
       <c r="V124">
         <v>111000</v>
@@ -10968,8 +10969,8 @@
       <c r="T125">
         <v>-5.9</v>
       </c>
-      <c r="U125" t="s">
-        <v>177</v>
+      <c r="U125" s="15">
+        <v>3411472.29</v>
       </c>
       <c r="V125">
         <v>123000</v>
@@ -11048,8 +11049,8 @@
       <c r="T126">
         <v>12.4</v>
       </c>
-      <c r="U126" t="s">
-        <v>177</v>
+      <c r="U126" s="15">
+        <v>4401347.3099999996</v>
       </c>
       <c r="V126">
         <v>121000</v>
@@ -11128,8 +11129,8 @@
       <c r="T127">
         <v>-5.4</v>
       </c>
-      <c r="U127" t="s">
-        <v>177</v>
+      <c r="U127" s="15">
+        <v>5292478.57</v>
       </c>
       <c r="V127">
         <v>118000</v>
@@ -11208,8 +11209,8 @@
       <c r="T128">
         <v>5.4</v>
       </c>
-      <c r="U128" t="s">
-        <v>177</v>
+      <c r="U128" s="15">
+        <v>5923904.8300000001</v>
       </c>
       <c r="V128">
         <v>113000</v>
@@ -11288,8 +11289,8 @@
       <c r="T129">
         <v>-5.3</v>
       </c>
-      <c r="U129" t="s">
-        <v>177</v>
+      <c r="U129" s="15">
+        <v>7030944.4699999997</v>
       </c>
       <c r="V129">
         <v>103000</v>
@@ -11368,8 +11369,8 @@
       <c r="T130">
         <v>27.3</v>
       </c>
-      <c r="U130" t="s">
-        <v>177</v>
+      <c r="U130" s="15">
+        <v>7938994.1799999997</v>
       </c>
       <c r="V130">
         <v>102000</v>
@@ -11448,8 +11449,8 @@
       <c r="T131">
         <v>-29.5</v>
       </c>
-      <c r="U131" t="s">
-        <v>177</v>
+      <c r="U131" s="15">
+        <v>9901760.1400000006</v>
       </c>
       <c r="V131">
         <v>69800</v>
@@ -11528,8 +11529,8 @@
       <c r="T132">
         <v>-20.5</v>
       </c>
-      <c r="U132" t="s">
-        <v>177</v>
+      <c r="U132" s="15">
+        <v>10856319.77</v>
       </c>
       <c r="V132">
         <v>88500</v>
@@ -11608,8 +11609,8 @@
       <c r="T133">
         <v>77.099999999999994</v>
       </c>
-      <c r="U133" t="s">
-        <v>177</v>
+      <c r="U133" s="15">
+        <v>16625485.720000001</v>
       </c>
       <c r="V133">
         <v>107000</v>
@@ -11688,8 +11689,8 @@
       <c r="T134">
         <v>-12</v>
       </c>
-      <c r="U134" t="s">
-        <v>178</v>
+      <c r="U134" s="15">
+        <v>1495367.34</v>
       </c>
       <c r="V134">
         <v>109000</v>
@@ -11768,8 +11769,8 @@
       <c r="T135">
         <v>-0.2</v>
       </c>
-      <c r="U135" t="s">
-        <v>178</v>
+      <c r="U135" s="15">
+        <v>2742266.93</v>
       </c>
       <c r="V135">
         <v>122000</v>
@@ -11848,8 +11849,8 @@
       <c r="T136">
         <v>4.8</v>
       </c>
-      <c r="U136" t="s">
-        <v>178</v>
+      <c r="U136" s="15">
+        <v>3074116.59</v>
       </c>
       <c r="V136">
         <v>140000</v>
@@ -11928,8 +11929,8 @@
       <c r="T137">
         <v>10.8</v>
       </c>
-      <c r="U137" t="s">
-        <v>178</v>
+      <c r="U137" s="13">
+        <v>4592940.5</v>
       </c>
       <c r="V137">
         <v>129000</v>
@@ -12008,8 +12009,8 @@
       <c r="T138">
         <v>-15.2</v>
       </c>
-      <c r="U138" t="s">
-        <v>178</v>
+      <c r="U138" s="15">
+        <v>5699314.1799999997</v>
       </c>
       <c r="V138">
         <v>117000</v>
@@ -12088,8 +12089,8 @@
       <c r="T139">
         <v>-8.9</v>
       </c>
-      <c r="U139" t="s">
-        <v>178</v>
+      <c r="U139" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="V139">
         <v>96400</v>
@@ -12168,8 +12169,8 @@
       <c r="T140">
         <v>2.8</v>
       </c>
-      <c r="U140" t="s">
-        <v>178</v>
+      <c r="U140" s="15">
+        <v>8318802.79</v>
       </c>
       <c r="V140">
         <v>81500</v>
@@ -12248,8 +12249,8 @@
       <c r="T141">
         <v>-22.2</v>
       </c>
-      <c r="U141" t="s">
-        <v>178</v>
+      <c r="U141" s="15">
+        <v>8492996.6999999993</v>
       </c>
       <c r="V141">
         <v>74900</v>
@@ -12328,8 +12329,8 @@
       <c r="T142">
         <v>94</v>
       </c>
-      <c r="U142" t="s">
-        <v>178</v>
+      <c r="U142" s="15">
+        <v>12203979.98</v>
       </c>
       <c r="V142">
         <v>68500</v>
@@ -12408,8 +12409,8 @@
       <c r="T143">
         <v>-50.8</v>
       </c>
-      <c r="U143" t="s">
-        <v>178</v>
+      <c r="U143" s="15">
+        <v>13093092.5</v>
       </c>
       <c r="V143">
         <v>49900</v>
@@ -12488,8 +12489,8 @@
       <c r="T144">
         <v>-7.2</v>
       </c>
-      <c r="U144" t="s">
-        <v>178</v>
+      <c r="U144" s="15">
+        <v>16619240.5</v>
       </c>
       <c r="V144">
         <v>70600</v>
@@ -12568,8 +12569,8 @@
       <c r="T145">
         <v>93.9</v>
       </c>
-      <c r="U145" t="s">
-        <v>178</v>
+      <c r="U145" s="15">
+        <v>21319818.539999999</v>
       </c>
       <c r="V145">
         <v>60400</v>
@@ -12648,8 +12649,8 @@
       <c r="T146">
         <v>-27.3</v>
       </c>
-      <c r="U146" t="s">
-        <v>179</v>
+      <c r="U146" s="15">
+        <v>390051.6</v>
       </c>
       <c r="V146">
         <v>56700</v>
@@ -12728,8 +12729,8 @@
       <c r="T147">
         <v>2.6</v>
       </c>
-      <c r="U147" t="s">
-        <v>179</v>
+      <c r="U147" s="15">
+        <v>1936275.95</v>
       </c>
       <c r="V147">
         <v>51700</v>
@@ -12808,8 +12809,8 @@
       <c r="T148">
         <v>-72.8</v>
       </c>
-      <c r="U148" t="s">
-        <v>179</v>
+      <c r="U148" s="15">
+        <v>2781319.21</v>
       </c>
       <c r="V148">
         <v>46800</v>
@@ -12885,8 +12886,8 @@
       <c r="T149">
         <v>0</v>
       </c>
-      <c r="U149" t="s">
-        <v>179</v>
+      <c r="U149" s="15">
+        <v>3879519.85</v>
       </c>
       <c r="V149">
         <v>0</v>

</xml_diff>